<commit_message>
Sistemato download dati SA3
</commit_message>
<xml_diff>
--- a/lista_impianti.xlsx
+++ b/lista_impianti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Geronazzo\ownCloud - david.geronazzo@zilioenvironment.com@cloud.ziliogroup.com\DATI_CENTRALI_ZILIO\Database_Produzione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefano Trevisan\PycharmProjects\ilMatematico\ilMatematico3\ilMatematico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC086D4-82FD-4DEB-B581-F53DFC40A250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0492053E-B063-4F48-92C0-024F859D3D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2400" windowWidth="19605" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1695" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
   <si>
     <t>nome_impianto</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>CSTlast24hTL</t>
+  </si>
+  <si>
+    <t>Zilio_Roof/Zilio Group</t>
   </si>
 </sst>
 </file>
@@ -692,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +713,7 @@
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
@@ -807,6 +810,9 @@
       <c r="H2" s="2">
         <v>43570</v>
       </c>
+      <c r="M2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">

</xml_diff>